<commit_message>
Refactored macro hotkey logic to use add_hotkey/remove_hotkey with suppress=True to prevent KeyErrors
- Replaced unblock_key/unhook with add_hotkey/remove_hotkey for better control
- Fixed KeyError on stop_macro due to improper key unhooking
- Ensured hotkeys are suppressed to avoid unwanted key propagation
- Improved UI status updates and exception handling
- Added log support for better debugging
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Py-Project\ExcelCommandExecutor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0435B44-8E66-4925-9A44-360196D2AE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340B1218-71E7-4C65-99DB-03DAB13F0E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="18900" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Key</t>
   </si>
@@ -31,34 +31,49 @@
     <t>Action Type</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
     <t>write</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>ctrl+v</t>
-  </si>
-  <si>
     <t>hotkey</t>
   </si>
   <si>
-    <t>esc</t>
-  </si>
-  <si>
-    <t>exit</t>
+    <t>JUNK FOOD NIGHT</t>
+  </si>
+  <si>
+    <t>TROJAN HORSE FOR SALE</t>
+  </si>
+  <si>
+    <t>ATM OF EREBUS</t>
+  </si>
+  <si>
+    <t>LAY OF THE LAND</t>
+  </si>
+  <si>
+    <t>NINJACONNOR</t>
+  </si>
+  <si>
+    <t>WRATH OF THE GODS</t>
+  </si>
+  <si>
+    <t>Get the Lightning Storm, Earthquake, Meteor and Tornado god powers</t>
+  </si>
+  <si>
+    <t>1000 gold</t>
+  </si>
+  <si>
+    <t> 1000 wood</t>
+  </si>
+  <si>
+    <t>1000 food</t>
+  </si>
+  <si>
+    <t>Show map</t>
+  </si>
+  <si>
+    <t>100,000 each resource, maxes population cap, unlimited god power castings, 100x build/research speeds</t>
   </si>
 </sst>
 </file>
@@ -107,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,9 +132,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,18 +413,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.75" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="88.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.75" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -429,67 +442,99 @@
       <c r="E1"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="D2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B3"/>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
@@ -499,8 +544,19 @@
       <c r="D8"/>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="4"/>
+    <row r="9" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>